<commit_message>
add htn db for malawi
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_hypertension.xlsx
+++ b/tests/frameworks/framework_hypertension.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09C1A7D-BB77-4C46-8C92-93EBB3551EB5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B937AF06-B83F-7B46-A1C1-1DBA32919F58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="14180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Parameters" sheetId="6" r:id="rId5"/>
     <sheet name="Cascades" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -988,7 +988,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
   <si>
     <t>Code Name</t>
   </si>
@@ -1071,9 +1071,6 @@
     <t>Currently treated</t>
   </si>
   <si>
-    <t>dx, tx</t>
-  </si>
-  <si>
     <t>all_dx</t>
   </si>
   <si>
@@ -1134,9 +1131,6 @@
     <t>num_initiate/dx</t>
   </si>
   <si>
-    <t>num_loss</t>
-  </si>
-  <si>
     <t>num_loss/tx</t>
   </si>
   <si>
@@ -1146,9 +1140,6 @@
     <t>Annual number newly initiated onto treatment</t>
   </si>
   <si>
-    <t>Annual number lost to follow-up</t>
-  </si>
-  <si>
     <t>scr</t>
   </si>
   <si>
@@ -1164,12 +1155,6 @@
     <t>Screened people</t>
   </si>
   <si>
-    <t>scr, dx, tx</t>
-  </si>
-  <si>
-    <t>undx, scr, dx, tx</t>
-  </si>
-  <si>
     <t>num_screen</t>
   </si>
   <si>
@@ -1183,6 +1168,48 @@
   </si>
   <si>
     <t>num_diag/scr</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>Controlled</t>
+  </si>
+  <si>
+    <t>all_con</t>
+  </si>
+  <si>
+    <t>undx, scr, dx, tx, con</t>
+  </si>
+  <si>
+    <t>scr, dx, tx, con</t>
+  </si>
+  <si>
+    <t>dx, tx, con</t>
+  </si>
+  <si>
+    <t>tx, con</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>fail_rate</t>
+  </si>
+  <si>
+    <t>Treatment failure rate</t>
+  </si>
+  <si>
+    <t>Blood pressure controlled</t>
+  </si>
+  <si>
+    <t>Time after initiating treatment to achieve BP control (years)</t>
+  </si>
+  <si>
+    <t>cont_rate</t>
+  </si>
+  <si>
+    <t>Prevalent</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1247,7 +1274,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1264,7 +1291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1615,61 +1642,61 @@
       <selection activeCell="A3" sqref="A3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
@@ -1681,24 +1708,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+    <sheetView zoomScale="166" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1718,13 +1745,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1748,12 +1775,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1772,7 +1799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1796,7 +1823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1820,12 +1847,36 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E6" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1836,15 +1887,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
@@ -1861,26 +1912,30 @@
         <f>Compartments!$A$5</f>
         <v>tx</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="str">
+        <f>Compartments!$A$6</f>
+        <v>con</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>Compartments!$A$3</f>
         <v>scr</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>Compartments!$A$4</f>
         <v>dx</v>
@@ -1889,13 +1944,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>Compartments!$A$5</f>
         <v>tx</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="str">
+        <f>Compartments!$A$6</f>
+        <v>con</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1905,21 +1975,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1936,21 +2006,21 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1959,21 +2029,21 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1982,21 +2052,21 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -2005,21 +2075,21 @@
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -2028,15 +2098,38 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2047,27 +2140,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2096,21 +2189,21 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
@@ -2126,18 +2219,18 @@
         <v>7</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
@@ -2147,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>8</v>
@@ -2158,15 +2251,15 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -2182,18 +2275,18 @@
         <v>7</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
@@ -2203,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>8</v>
@@ -2214,15 +2307,15 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2">
@@ -2238,18 +2331,18 @@
         <v>7</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="2">
@@ -2259,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>8</v>
@@ -2270,76 +2363,98 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.2</v>
+      </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2350,7 +2465,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2361,7 +2476,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2372,7 +2487,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2383,7 +2498,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2394,7 +2509,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2405,7 +2520,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2416,7 +2531,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2427,7 +2542,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2438,7 +2553,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2449,23 +2564,12 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10 H2:I21" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I20 J2:J10" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>",number,probability,duration,proportion"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2477,56 +2581,64 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5680499-D84A-1B4F-B644-03899BDE28FE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="179" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>